<commit_message>
Added DB test results to Results.xlsx
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -9,22 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11895" tabRatio="570" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11895" tabRatio="570" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Latest (Pivot)" sheetId="5" r:id="rId1"/>
-    <sheet name="Latest" sheetId="4" r:id="rId2"/>
-    <sheet name="Plaintext" sheetId="8" r:id="rId3"/>
-    <sheet name="JSON" sheetId="9" r:id="rId4"/>
+    <sheet name="Plaintext" sheetId="8" r:id="rId1"/>
+    <sheet name="JSON" sheetId="9" r:id="rId2"/>
+    <sheet name="Single query" sheetId="10" r:id="rId3"/>
+    <sheet name="Multiple queries" sheetId="11" r:id="rId4"/>
+    <sheet name="Fortunes" sheetId="12" r:id="rId5"/>
+    <sheet name="Latest (Pivot)" sheetId="5" r:id="rId6"/>
+    <sheet name="Latest" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">JSON!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Latest!$A$1:$U$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Plaintext!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Fortunes!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">JSON!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Latest!$A$1:$U$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Multiple queries'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plaintext!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Single query'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +46,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +121,72 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>8 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>16 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>32 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>64 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>128 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,10 +208,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1,024 concurrency</t>
+          <t>Best performance across all concurrency levels</t>
         </r>
       </text>
     </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Damian Edwards</author>
+  </authors>
+  <commentList>
     <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -150,7 +231,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>4.096 concurrency</t>
+          <t>8 concurrency</t>
         </r>
       </text>
     </comment>
@@ -163,11 +244,239 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>16,384 concurrency</t>
+          <t>16 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>32 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>64 concurrency</t>
         </r>
       </text>
     </comment>
     <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>128 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>256 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Best performance across all concurrency levels</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Damian Edwards</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 query/request</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 queries/request</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10 queries/request</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>15 queries/request</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>20 queries/request</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Damian Edwards</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>8 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>16 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>32 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>64 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>128 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>128 concurrency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -342,6 +651,36 @@
   <si>
     <t>x65</t>
   </si>
+  <si>
+    <t>ORM</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>SQL Server 2014</t>
+  </si>
+  <si>
+    <t>Raw ADO.NET</t>
+  </si>
+  <si>
+    <t>Dapper</t>
+  </si>
+  <si>
+    <t>EF 7</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Raw middleware</t>
+  </si>
+  <si>
+    <t>JSON Library</t>
+  </si>
+  <si>
+    <t>JSON.NET</t>
+  </si>
 </sst>
 </file>
 
@@ -434,168 +773,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3759,7 +3937,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
   <location ref="A5:E19" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -4242,6 +4420,1280 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="8" style="9" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9" style="9" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="12">
+        <v>256</v>
+      </c>
+      <c r="H1" s="12">
+        <v>1024</v>
+      </c>
+      <c r="I1" s="12">
+        <v>4096</v>
+      </c>
+      <c r="J1" s="12">
+        <v>16384</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42256</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="13">
+        <v>391000</v>
+      </c>
+      <c r="K2" s="13">
+        <f>MAX(G2:J2)</f>
+        <v>391000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42272</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="13">
+        <v>391000</v>
+      </c>
+      <c r="K3" s="13">
+        <f t="shared" ref="K3:K14" si="0">MAX(G3:J3)</f>
+        <v>391000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42277</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="13">
+        <v>391000</v>
+      </c>
+      <c r="K4" s="13">
+        <f t="shared" si="0"/>
+        <v>391000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="13">
+        <v>66862</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="K5" s="13">
+        <f t="shared" si="0"/>
+        <v>66862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42285</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
+        <v>221495</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="0"/>
+        <v>221495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="13">
+        <v>443083</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" si="0"/>
+        <v>443083</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42286</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="13">
+        <v>123808</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" ref="K8" si="1">MAX(G8:J8)</f>
+        <v>123808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42286</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="13">
+        <v>319007</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="0"/>
+        <v>319007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42314</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="13">
+        <v>409856</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="0"/>
+        <v>409856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42314</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="13">
+        <v>505350</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="0"/>
+        <v>505350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="13">
+        <v>390420</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="0"/>
+        <v>390420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="13">
+        <v>491496</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" si="0"/>
+        <v>491496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42333</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="9">
+        <v>738279</v>
+      </c>
+      <c r="H14" s="13">
+        <v>743123</v>
+      </c>
+      <c r="I14" s="9">
+        <v>724844</v>
+      </c>
+      <c r="J14" s="9">
+        <v>713901</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="0"/>
+        <v>743123</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1">
+    <sortState ref="A2:J13">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="8" style="9" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="9" customWidth="1"/>
+    <col min="11" max="13" width="9" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="12">
+        <v>8</v>
+      </c>
+      <c r="I1" s="12">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12">
+        <v>32</v>
+      </c>
+      <c r="K1" s="12">
+        <v>64</v>
+      </c>
+      <c r="L1" s="12">
+        <v>128</v>
+      </c>
+      <c r="M1" s="12">
+        <v>256</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42286</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="L2" s="9">
+        <v>64669</v>
+      </c>
+      <c r="N2" s="13">
+        <f>MAX(H2:M2)</f>
+        <v>64669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="M3" s="9">
+        <v>66854</v>
+      </c>
+      <c r="N3" s="13">
+        <f t="shared" ref="N3:N6" si="0">MAX(H3:M3)</f>
+        <v>66854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="M4" s="9">
+        <v>131819</v>
+      </c>
+      <c r="N4" s="13">
+        <f t="shared" si="0"/>
+        <v>131819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="M5" s="9">
+        <v>146894</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" si="0"/>
+        <v>146894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42333</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="9">
+        <v>63530</v>
+      </c>
+      <c r="I6" s="9">
+        <v>99050</v>
+      </c>
+      <c r="J6" s="9">
+        <v>129971</v>
+      </c>
+      <c r="K6" s="9">
+        <v>148262</v>
+      </c>
+      <c r="L6" s="9">
+        <v>156589</v>
+      </c>
+      <c r="M6" s="9">
+        <v>161392</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="0"/>
+        <v>161392</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N1">
+    <sortState ref="A2:J13">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="12">
+        <v>8</v>
+      </c>
+      <c r="I1" s="12">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12">
+        <v>32</v>
+      </c>
+      <c r="K1" s="12">
+        <v>64</v>
+      </c>
+      <c r="L1" s="12">
+        <v>128</v>
+      </c>
+      <c r="M1" s="12">
+        <v>256</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="9">
+        <v>10748</v>
+      </c>
+      <c r="I2" s="9">
+        <v>19233</v>
+      </c>
+      <c r="J2" s="9">
+        <v>23482</v>
+      </c>
+      <c r="K2" s="9">
+        <v>23843</v>
+      </c>
+      <c r="L2" s="9">
+        <v>23624</v>
+      </c>
+      <c r="M2" s="9">
+        <v>24301</v>
+      </c>
+      <c r="N2" s="13">
+        <f t="shared" ref="N2" si="0">MAX(H2:M2)</f>
+        <v>24301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="9">
+        <v>10547</v>
+      </c>
+      <c r="I3" s="9">
+        <v>18570</v>
+      </c>
+      <c r="J3" s="9">
+        <v>22397</v>
+      </c>
+      <c r="K3" s="9">
+        <v>22730</v>
+      </c>
+      <c r="L3" s="9">
+        <v>22747</v>
+      </c>
+      <c r="M3" s="9">
+        <v>22808</v>
+      </c>
+      <c r="N3" s="13">
+        <f t="shared" ref="N3:N4" si="1">MAX(H3:M3)</f>
+        <v>22808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="9">
+        <v>8994</v>
+      </c>
+      <c r="I4" s="9">
+        <v>12607</v>
+      </c>
+      <c r="J4" s="9">
+        <v>17897</v>
+      </c>
+      <c r="K4" s="9">
+        <v>18197</v>
+      </c>
+      <c r="L4" s="9">
+        <v>17812</v>
+      </c>
+      <c r="M4" s="9">
+        <v>17957</v>
+      </c>
+      <c r="N4" s="13">
+        <f t="shared" si="1"/>
+        <v>18197</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="12">
+        <v>1</v>
+      </c>
+      <c r="I1" s="12">
+        <v>5</v>
+      </c>
+      <c r="J1" s="12">
+        <v>10</v>
+      </c>
+      <c r="K1" s="12">
+        <v>15</v>
+      </c>
+      <c r="L1" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="9">
+        <v>22478</v>
+      </c>
+      <c r="I2" s="9">
+        <v>4667</v>
+      </c>
+      <c r="J2" s="9">
+        <v>2344</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1553</v>
+      </c>
+      <c r="L2" s="9">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="9">
+        <v>22237</v>
+      </c>
+      <c r="I3" s="9">
+        <v>4600</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2309</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1534</v>
+      </c>
+      <c r="L3" s="9">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="9">
+        <v>16846</v>
+      </c>
+      <c r="I4" s="9">
+        <v>3961</v>
+      </c>
+      <c r="J4" s="9">
+        <v>2023</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1340</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1001</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="12">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12">
+        <v>16</v>
+      </c>
+      <c r="K1" s="12">
+        <v>32</v>
+      </c>
+      <c r="L1" s="12">
+        <v>64</v>
+      </c>
+      <c r="M1" s="12">
+        <v>128</v>
+      </c>
+      <c r="N1" s="12">
+        <v>256</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="9">
+        <v>9575</v>
+      </c>
+      <c r="J2" s="9">
+        <v>14168</v>
+      </c>
+      <c r="K2" s="9">
+        <v>19034</v>
+      </c>
+      <c r="L2" s="9">
+        <v>20058</v>
+      </c>
+      <c r="M2" s="9">
+        <v>20137</v>
+      </c>
+      <c r="N2" s="9">
+        <v>19385</v>
+      </c>
+      <c r="O2" s="13">
+        <f t="shared" ref="O2:O4" si="0">MAX(I2:N2)</f>
+        <v>20137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="9">
+        <v>9441</v>
+      </c>
+      <c r="J3" s="9">
+        <v>14099</v>
+      </c>
+      <c r="K3" s="9">
+        <v>19365</v>
+      </c>
+      <c r="L3" s="9">
+        <v>19564</v>
+      </c>
+      <c r="M3" s="9">
+        <v>18836</v>
+      </c>
+      <c r="N3" s="9">
+        <v>19293</v>
+      </c>
+      <c r="O3" s="13">
+        <f t="shared" si="0"/>
+        <v>19564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="9">
+        <v>6949</v>
+      </c>
+      <c r="J4" s="9">
+        <v>10565</v>
+      </c>
+      <c r="K4" s="9">
+        <v>14082</v>
+      </c>
+      <c r="L4" s="9">
+        <v>14858</v>
+      </c>
+      <c r="M4" s="9">
+        <v>14730</v>
+      </c>
+      <c r="N4" s="9">
+        <v>14287</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" si="0"/>
+        <v>14858</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
@@ -4485,7 +5937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U17"/>
@@ -5157,604 +6609,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8" style="9" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9" style="9" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="12">
-        <v>256</v>
-      </c>
-      <c r="G1" s="12">
-        <v>1024</v>
-      </c>
-      <c r="H1" s="12">
-        <v>4096</v>
-      </c>
-      <c r="I1" s="12">
-        <v>16384</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42256</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="13">
-        <v>391000</v>
-      </c>
-      <c r="J2" s="13">
-        <f>MAX(F2:I2)</f>
-        <v>391000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42272</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="13">
-        <v>391000</v>
-      </c>
-      <c r="J3" s="13">
-        <f t="shared" ref="J3:J14" si="0">MAX(F3:I3)</f>
-        <v>391000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42277</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="13">
-        <v>391000</v>
-      </c>
-      <c r="J4" s="13">
-        <f t="shared" si="0"/>
-        <v>391000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42285</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="13">
-        <v>66862</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="J5" s="13">
-        <f t="shared" si="0"/>
-        <v>66862</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13">
-        <v>221495</v>
-      </c>
-      <c r="J6" s="13">
-        <f t="shared" si="0"/>
-        <v>221495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>42285</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="13">
-        <v>443083</v>
-      </c>
-      <c r="J7" s="13">
-        <f t="shared" si="0"/>
-        <v>443083</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>42286</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="13">
-        <v>123808</v>
-      </c>
-      <c r="J8" s="13">
-        <f t="shared" ref="J8" si="1">MAX(F8:I8)</f>
-        <v>123808</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>42286</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="13">
-        <v>319007</v>
-      </c>
-      <c r="J9" s="13">
-        <f t="shared" si="0"/>
-        <v>319007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>42314</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="13">
-        <v>409856</v>
-      </c>
-      <c r="J10" s="13">
-        <f t="shared" si="0"/>
-        <v>409856</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>42314</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="13">
-        <v>505350</v>
-      </c>
-      <c r="J11" s="13">
-        <f t="shared" si="0"/>
-        <v>505350</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>42317</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="13">
-        <v>390420</v>
-      </c>
-      <c r="J12" s="13">
-        <f t="shared" si="0"/>
-        <v>390420</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>42317</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="13">
-        <v>491496</v>
-      </c>
-      <c r="J13" s="13">
-        <f t="shared" si="0"/>
-        <v>491496</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>42333</v>
-      </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="9">
-        <v>738279</v>
-      </c>
-      <c r="G14" s="13">
-        <v>743123</v>
-      </c>
-      <c r="H14" s="9">
-        <v>724844</v>
-      </c>
-      <c r="I14" s="9">
-        <v>713901</v>
-      </c>
-      <c r="J14" s="13">
-        <f t="shared" si="0"/>
-        <v>743123</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J1">
-    <sortState ref="A2:J13">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8" style="9" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="9" customWidth="1"/>
-    <col min="9" max="11" width="9" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="12">
-        <v>8</v>
-      </c>
-      <c r="G1" s="12">
-        <v>16</v>
-      </c>
-      <c r="H1" s="12">
-        <v>32</v>
-      </c>
-      <c r="I1" s="12">
-        <v>64</v>
-      </c>
-      <c r="J1" s="12">
-        <v>128</v>
-      </c>
-      <c r="K1" s="12">
-        <v>256</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42286</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="J2" s="9">
-        <v>64669</v>
-      </c>
-      <c r="L2" s="13">
-        <f>MAX(F2:K2)</f>
-        <v>64669</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42286</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="K3" s="9">
-        <v>66854</v>
-      </c>
-      <c r="L3" s="13">
-        <f t="shared" ref="L3:L6" si="0">MAX(F3:K3)</f>
-        <v>66854</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>42317</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="K4" s="9">
-        <v>131819</v>
-      </c>
-      <c r="L4" s="13">
-        <f t="shared" si="0"/>
-        <v>131819</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>42317</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="K5" s="9">
-        <v>146894</v>
-      </c>
-      <c r="L5" s="13">
-        <f t="shared" si="0"/>
-        <v>146894</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>42333</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="9">
-        <v>63530</v>
-      </c>
-      <c r="G6" s="9">
-        <v>99050</v>
-      </c>
-      <c r="H6" s="9">
-        <v>129971</v>
-      </c>
-      <c r="I6" s="9">
-        <v>148262</v>
-      </c>
-      <c r="J6" s="9">
-        <v>156589</v>
-      </c>
-      <c r="K6" s="9">
-        <v>161392</v>
-      </c>
-      <c r="L6" s="13">
-        <f t="shared" si="0"/>
-        <v>161392</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:L1">
-    <sortState ref="A2:J13">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated plaintext results for Windows
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\src\GitHub\aspnet\benchmarks\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\GitHub\aspnet\benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11895" tabRatio="570" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11900" tabRatio="570"/>
   </bookViews>
   <sheets>
     <sheet name="Plaintext" sheetId="8" r:id="rId1"/>
@@ -494,7 +494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -4421,27 +4421,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="8" style="9" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9" style="9" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="9" customWidth="1"/>
+    <col min="7" max="11" width="8.7265625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4476,7 +4472,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42256</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>391000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42272</v>
       </c>
@@ -4526,11 +4522,11 @@
         <v>391000</v>
       </c>
       <c r="K3" s="13">
-        <f t="shared" ref="K3:K14" si="0">MAX(G3:J3)</f>
+        <f t="shared" ref="K3:K15" si="0">MAX(G3:J3)</f>
         <v>391000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42277</v>
       </c>
@@ -4557,7 +4553,7 @@
         <v>391000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42285</v>
       </c>
@@ -4585,7 +4581,7 @@
         <v>66862</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42285</v>
       </c>
@@ -4613,7 +4609,7 @@
         <v>221495</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>42285</v>
       </c>
@@ -4640,7 +4636,7 @@
         <v>443083</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42286</v>
       </c>
@@ -4667,7 +4663,7 @@
         <v>123808</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>42286</v>
       </c>
@@ -4694,7 +4690,7 @@
         <v>319007</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>42314</v>
       </c>
@@ -4721,7 +4717,7 @@
         <v>409856</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>42314</v>
       </c>
@@ -4748,7 +4744,7 @@
         <v>505350</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>42317</v>
       </c>
@@ -4775,7 +4771,7 @@
         <v>390420</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>42317</v>
       </c>
@@ -4802,7 +4798,7 @@
         <v>491496</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>42333</v>
       </c>
@@ -4836,6 +4832,42 @@
       <c r="K14" s="13">
         <f t="shared" si="0"/>
         <v>743123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>42395</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1188521</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1182663</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1169144</v>
+      </c>
+      <c r="J15" s="9">
+        <v>1145456</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="0"/>
+        <v>1188521</v>
       </c>
     </row>
   </sheetData>
@@ -4858,22 +4890,22 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" style="9" customWidth="1"/>
     <col min="9" max="9" width="8" style="9" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" style="9" customWidth="1"/>
     <col min="11" max="13" width="9" style="9" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.1796875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4917,7 +4949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42286</v>
       </c>
@@ -4949,7 +4981,7 @@
         <v>64669</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42286</v>
       </c>
@@ -4981,7 +5013,7 @@
         <v>66854</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42317</v>
       </c>
@@ -5012,7 +5044,7 @@
         <v>131819</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>42317</v>
       </c>
@@ -5043,7 +5075,7 @@
         <v>146894</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>42333</v>
       </c>
@@ -5108,15 +5140,15 @@
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5160,7 +5192,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42338</v>
       </c>
@@ -5205,7 +5237,7 @@
         <v>24301</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42338</v>
       </c>
@@ -5250,7 +5282,7 @@
         <v>22808</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42338</v>
       </c>
@@ -5310,15 +5342,15 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5356,7 +5388,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42338</v>
       </c>
@@ -5394,7 +5426,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42338</v>
       </c>
@@ -5432,7 +5464,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42338</v>
       </c>
@@ -5482,19 +5514,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5541,7 +5573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>42338</v>
       </c>
@@ -5589,7 +5621,7 @@
         <v>20137</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42338</v>
       </c>
@@ -5637,7 +5669,7 @@
         <v>19564</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>42338</v>
       </c>
@@ -5701,28 +5733,28 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" customWidth="1"/>
     <col min="12" max="12" width="7" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" customWidth="1"/>
     <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.54296875" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -5730,7 +5762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5738,7 +5770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -5746,7 +5778,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1</v>
       </c>
@@ -5754,7 +5786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -5771,7 +5803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -5788,7 +5820,7 @@
         <v>51290</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -5805,7 +5837,7 @@
         <v>51290</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -5816,7 +5848,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -5827,7 +5859,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5840,7 +5872,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
@@ -5853,7 +5885,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -5866,7 +5898,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -5879,7 +5911,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -5892,7 +5924,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
@@ -5905,7 +5937,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
@@ -5918,7 +5950,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
@@ -5946,30 +5978,30 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.54296875" customWidth="1"/>
+    <col min="21" max="21" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -6034,7 +6066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -6069,7 +6101,7 @@
         <v>51379</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6104,7 +6136,7 @@
         <v>66854</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -6139,7 +6171,7 @@
         <v>51290</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -6174,7 +6206,7 @@
         <v>57843</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -6209,7 +6241,7 @@
         <v>57792</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -6244,7 +6276,7 @@
         <v>168005</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6279,7 +6311,7 @@
         <v>102730</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6314,7 +6346,7 @@
         <v>123808</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -6349,7 +6381,7 @@
         <v>124262</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -6384,7 +6416,7 @@
         <v>131519</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -6419,7 +6451,7 @@
         <v>176509</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -6454,7 +6486,7 @@
         <v>390420</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -6489,7 +6521,7 @@
         <v>743123</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -6524,7 +6556,7 @@
         <v>1514942</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -6559,7 +6591,7 @@
         <v>447993</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update README.md & results
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -4431,7 +4431,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,7 +4441,7 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="11" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Linux plaintext pipelining results of January 13th in the excel document.
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\src\GitHub\aspnet\benchmarks\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11895" tabRatio="570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="570"/>
   </bookViews>
   <sheets>
     <sheet name="Plaintext" sheetId="8" r:id="rId1"/>
@@ -28,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plaintext!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Single query'!$A$1:$N$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
@@ -46,7 +41,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +116,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +217,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -274,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +318,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -375,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -398,7 +393,7 @@
     <author>Damian Edwards</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -411,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -437,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -450,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -476,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +489,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -682,15 +677,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -698,14 +693,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -718,8 +713,15 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -742,7 +744,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -767,11 +769,39 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="千分位" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -784,9 +814,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -838,7 +868,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -902,7 +932,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-TW"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -911,7 +941,7 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
@@ -1025,7 +1055,7 @@
         <c:idx val="9"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent3"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -1040,7 +1070,22 @@
         <c:idx val="10"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -1157,7 +1202,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C2B8-4359-9B43-7DD91AC40764}"/>
             </c:ext>
@@ -1247,7 +1292,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C2B8-4359-9B43-7DD91AC40764}"/>
             </c:ext>
@@ -1349,7 +1394,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-C2B8-4359-9B43-7DD91AC40764}"/>
             </c:ext>
@@ -1439,7 +1484,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-C2B8-4359-9B43-7DD91AC40764}"/>
             </c:ext>
@@ -1455,11 +1500,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="545828712"/>
-        <c:axId val="478992168"/>
+        <c:axId val="271237120"/>
+        <c:axId val="271238656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="545828712"/>
+        <c:axId val="271237120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,10 +1544,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478992168"/>
+        <c:crossAx val="271238656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1510,7 +1555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="478992168"/>
+        <c:axId val="271238656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,10 +1603,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545828712"/>
+        <c:crossAx val="271237120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1600,7 +1645,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1630,7 +1675,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1638,7 +1683,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:extLst>
+  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
@@ -1651,9 +1696,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1690,7 +1735,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-TW"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1749,7 +1794,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-TW"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -1760,7 +1805,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -2124,7 +2169,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-FEEB-41F9-921F-AD6E752578BD}"/>
             </c:ext>
@@ -2141,12 +2186,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="624117456"/>
-        <c:axId val="624119752"/>
-        <c:extLst/>
+        <c:axId val="271095296"/>
+        <c:axId val="271524224"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624117456"/>
+        <c:axId val="271095296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,10 +2231,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624119752"/>
+        <c:crossAx val="271524224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2197,7 +2242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624119752"/>
+        <c:axId val="271524224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,10 +2290,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624117456"/>
+        <c:crossAx val="271095296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2286,7 +2331,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4100,7 +4145,7 @@
   <dataFields count="1">
     <dataField name="Max of RPS Avg" fld="10" subtotal="max" baseField="0" baseItem="3"/>
   </dataFields>
-  <chartFormats count="4">
+  <chartFormats count="5">
     <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -4151,6 +4196,21 @@
           </reference>
           <reference field="9" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -4420,7 +4480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4428,13 +4488,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -4529,7 +4589,7 @@
         <v>391000</v>
       </c>
       <c r="K3" s="13">
-        <f t="shared" ref="K3:K15" si="0">MAX(G3:J3)</f>
+        <f t="shared" ref="K3:K16" si="0">MAX(G3:J3)</f>
         <v>391000</v>
       </c>
     </row>
@@ -4843,10 +4903,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>42395</v>
+        <v>42382</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -4861,18 +4921,45 @@
         <v>57</v>
       </c>
       <c r="G15" s="13">
+        <v>928023</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" ref="K15" si="2">MAX(G15:J15)</f>
+        <v>928023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42395</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="13">
         <v>1188521</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H16" s="9">
         <v>1182663</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I16" s="9">
         <v>1169144</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J16" s="9">
         <v>1145456</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K16" s="13">
         <f t="shared" si="0"/>
         <v>1188521</v>
       </c>
@@ -4883,6 +4970,7 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -4897,7 +4985,7 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -5178,6 +5266,7 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5192,7 +5281,7 @@
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
@@ -5381,6 +5470,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -5394,7 +5484,7 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
@@ -5556,6 +5646,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5570,7 +5661,7 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
@@ -5771,6 +5862,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5785,7 +5877,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
@@ -6024,6 +6116,7 @@
       <c r="E19" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -6038,7 +6131,7 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -6689,7 +6782,7 @@
   </sheetData>
   <autoFilter ref="A1:U17">
     <filterColumn colId="2">
-      <filters blank="1">
+      <filters>
         <filter val="plaintext"/>
       </filters>
     </filterColumn>
@@ -6697,6 +6790,7 @@
       <sortCondition ref="K1:K13"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>